<commit_message>
complete project commited with final code
</commit_message>
<xml_diff>
--- a/GroceryApplication/src/test/resources/Testdata/GroceryApp.xlsx
+++ b/GroceryApplication/src/test/resources/Testdata/GroceryApp.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0EDE9B17-84DC-4241-9E24-718AE0BAA8CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91828\git\AutomationMainProject\GroceryApplication\src\test\resources\Testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC99D33A-2375-4ADE-8102-8334508F0CD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="4836" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +17,6 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
@@ -33,13 +37,16 @@
     <t>admin</t>
   </si>
   <si>
-    <t>renjini</t>
-  </si>
-  <si>
     <t>tester</t>
   </si>
   <si>
-    <t>test123</t>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>sree</t>
+  </si>
+  <si>
+    <t>xyzabcjkl</t>
   </si>
 </sst>
 </file>
@@ -357,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,10 +394,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>12345</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -398,7 +405,15 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>